<commit_message>
Optimized the algorithm, fixed the parsing error for some special courses
</commit_message>
<xml_diff>
--- a/Scraping + Scheduling/calendar.xlsx
+++ b/Scraping + Scheduling/calendar.xlsx
@@ -542,7 +542,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['ARABL-UH 1120 - Elementary Arabic 2 is waitlisted. You are going to be number 0 in the queue. Be aware of that.']</t>
+          <t>['MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.', 'ARABL-UH 1120 - Elementary Arabic 2 is waitlisted. You are going to be number 0 in the queue. Be aware of that.']</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['ARABL-UH 1120 - Elementary Arabic 2 is waitlisted. You are going to be number 0 in the queue. Be aware of that.', 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.']</t>
+          <t>['MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.', 'ARABL-UH 1120 - Elementary Arabic 2 is waitlisted. You are going to be number 0 in the queue. Be aware of that.', 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed scheduling for fixed and unfixed courses
</commit_message>
<xml_diff>
--- a/Scraping + Scheduling/calendar.xlsx
+++ b/Scraping + Scheduling/calendar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +440,18 @@
       <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -447,12 +459,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '001-SEM (18450)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}, {'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '003-SEM (18353)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '001-SEM (18354)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh, Omima El Araby', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC1-RCT (18468)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}]</t>
+          <t>{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '001-SEM (18450)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>{'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '003-SEM (18353)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>{'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '001-SEM (18354)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh, Omima El Araby', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>{'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>{'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC1-RCT (18468)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}</t>
         </is>
       </c>
     </row>
@@ -462,12 +494,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '001-SEM (18450)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}, {'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '003-SEM (18353)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '001-SEM (18354)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh, Omima El Araby', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC2-RCT (18469)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Staff', 'status': 'Wait List', 'waitlist_count': '4', 'session': 'A71'}]</t>
+          <t>{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '001-SEM (18450)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.']</t>
+          <t>{'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '003-SEM (18353)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>{'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '001-SEM (18354)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh, Omima El Araby', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>{'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>{'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC2-RCT (18469)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Staff', 'status': 'Wait List', 'waitlist_count': '4', 'session': 'A71'}</t>
         </is>
       </c>
     </row>
@@ -477,12 +529,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '001-SEM (18450)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}, {'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '002-SEM (18021)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Wait List', 'waitlist_count': '0', 'session': 'AD'}, {'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '002-SEM (18786)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC1-RCT (18468)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}]</t>
+          <t>{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '001-SEM (18450)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['ARABL-UH 1120 - Elementary Arabic 2 is waitlisted. You are going to be number 0 in the queue. Be aware of that.']</t>
+          <t>{'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '002-SEM (18021)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Wait List', 'waitlist_count': '0', 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>{'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '002-SEM (18786)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>{'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>{'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC1-RCT (18468)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}</t>
         </is>
       </c>
     </row>
@@ -492,72 +564,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '001-SEM (18450)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}, {'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '002-SEM (18021)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Wait List', 'waitlist_count': '0', 'session': 'AD'}, {'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '002-SEM (18786)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC2-RCT (18469)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Staff', 'status': 'Wait List', 'waitlist_count': '4', 'session': 'A71'}]</t>
+          <t>{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '001-SEM (18450)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['ARABL-UH 1120 - Elementary Arabic 2 is waitlisted. You are going to be number 0 in the queue. Be aware of that.', 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.']</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>[{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '002-SEM (18467)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Weiren Zhao', 'status': 'Wait List', 'waitlist_count': '4', 'session': 'A71'}, {'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '003-SEM (18353)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '001-SEM (18354)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh, Omima El Araby', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC1-RCT (18468)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}]</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>['MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.']</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>[{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '002-SEM (18467)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Weiren Zhao', 'status': 'Wait List', 'waitlist_count': '4', 'session': 'A71'}, {'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '003-SEM (18353)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '001-SEM (18354)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh, Omima El Araby', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC2-RCT (18469)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Staff', 'status': 'Wait List', 'waitlist_count': '4', 'session': 'A71'}]</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>['MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.', 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.']</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>[{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '002-SEM (18467)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Weiren Zhao', 'status': 'Wait List', 'waitlist_count': '4', 'session': 'A71'}, {'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '002-SEM (18021)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Wait List', 'waitlist_count': '0', 'session': 'AD'}, {'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '002-SEM (18786)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC1-RCT (18468)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Dania Zantout', 'status': 'Open', 'waitlist_count': 0, 'session': 'A71'}]</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>['MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.', 'ARABL-UH 1120 - Elementary Arabic 2 is waitlisted. You are going to be number 0 in the queue. Be aware of that.']</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>[{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': '002-SEM (18467)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['T', 'R'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Weiren Zhao', 'status': 'Wait List', 'waitlist_count': '4', 'session': 'A71'}, {'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '002-SEM (18021)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Wait List', 'waitlist_count': '0', 'session': 'AD'}, {'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '002-SEM (18786)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}, {'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC2-RCT (18469)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Staff', 'status': 'Wait List', 'waitlist_count': '4', 'session': 'A71'}]</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>['MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.', 'ARABL-UH 1120 - Elementary Arabic 2 is waitlisted. You are going to be number 0 in the queue. Be aware of that.', 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I is waitlisted. You are going to be number 4 in the queue. Be aware of that.']</t>
+          <t>{'name': 'ARABL-UH 1120 - Elementary Arabic 2', 'title': '002-SEM (18021)', 'id': 'ARABLUH1120160332', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 10.416666666667, 'end_date': 11.666666666667, 'inscturct_mode': 'P', 'instructor': 'Muhamed Al-Khalil', 'status': 'Wait List', 'waitlist_count': '0', 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>{'name': 'ARABL-UH 2120 - Intermediate Arabic 2', 'title': '002-SEM (18786)', 'id': 'ARABLUH2120204522', 'term': '1224', 'campus': 'AD', 'days': ['M', 'T', 'W', 'R'], 'start_date': 11.833333333333, 'end_date': 13.083333333333, 'inscturct_mode': 'P', 'instructor': 'Khulood Kittaneh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>{'name': 'ARTH-UH 2128 - Money and Art in the Global Renaissance', 'title': '001-SEM (22629)', 'id': 'ARTHUH2128232572', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 13.25, 'end_date': 14.5, 'inscturct_mode': 'P', 'instructor': 'Mahnaz Yousefzadeh', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>{'name': 'AW-UH 1118 - Archaeology, Arabia and the Bible', 'title': '001-SEM (24761)', 'id': 'AWUH1118236369', 'term': '1224', 'campus': 'AD', 'days': ['M', 'W'], 'start_date': 14.666666666667, 'end_date': 15.916666666667, 'inscturct_mode': 'P', 'instructor': 'William Zimmerle', 'status': 'Open', 'waitlist_count': 0, 'session': 'AD'}</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>{'name': 'MATH-UH 1000A - Mathematics for Statistics and Calculus Part I', 'title': 'REC2-RCT (18469)', 'id': 'MATHUH1000A234160', 'term': '1224', 'campus': 'AD', 'days': ['U'], 'start_date': 9.0, 'end_date': 10.25, 'inscturct_mode': 'P', 'instructor': 'Staff', 'status': 'Wait List', 'waitlist_count': '4', 'session': 'A71'}</t>
         </is>
       </c>
     </row>

</xml_diff>